<commit_message>
addDropId 로 Id 붙임
Enum 들은 대문자로 시작
</commit_message>
<xml_diff>
--- a/Excel/Drop.xlsx
+++ b/Excel/Drop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A18A48-BDA9-48A8-8E1A-669D49C838AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C7DA33-D57C-44C7-9A70-CB8C1C6BF772}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B53FE973-D001-484E-B693-7C0DF00F159C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>dropId|String</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,20 +76,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Exp, Gold, Heart, Gacha</t>
+  </si>
+  <si>
     <t>,,,11001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1,1,1,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>15,16,1,2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>15,20,1,4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -453,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA9DE39-B717-40A9-BC21-70CAE1ED14B8}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,22 +509,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>5001</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D4" t="s">
         <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>